<commit_message>
New tests and sample files
</commit_message>
<xml_diff>
--- a/sample_input.xlsx
+++ b/sample_input.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="158">
   <si>
     <t xml:space="preserve">ДАТА</t>
   </si>
@@ -350,6 +350,153 @@
   </si>
   <si>
     <t xml:space="preserve">SUBARU XV 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EVA_BORT_Chery_Tiggo 5_I пок и R_2005-2016_black+12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHERY TIGGO 5 1 и рестайлинг</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VOD_Chery_Tiggo 5_I пок и R_2005-2016_black+12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EVA_BORT+Chery+Tigg_o7ProMBez+2020-2024+black+16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHERY TIGGO 7 без панорамы</t>
+  </si>
+  <si>
+    <t xml:space="preserve">без панорамы</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PERED_EVA+Chery+Tiggo 7 Pro Max+2020-2024+black+1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHERY TIGGO 7 панорама</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VOD+Chery+Tiggo_7ProMAXbeZ+2020-2024+black+11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EVA_BORT_Dodge_Nitro_I пок_2006-2011_black+12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DODGE NITRO 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EVA_BORT+Doodge+RAM+2008-2021+black+12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DODGE RAM 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EVA_BORT+Geely+Emgrand 7+2020-2022+black+12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GEELY EMGRAND 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EVA_BORT+Geely+Emgrand EC 7+2020-2023+black+12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GEELY EMGRAND 7 EC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VOD+Hyundai+Solaris+2010-2017 +black+11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HYUNDAI SOLARIS 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EVA_BORT+Hyundai+Sol_a_ris+2010-2017 +black+9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EVA_BORT+Hyundai+Solaris +2017-2022+black+11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HYUNDAI SOLARIS 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EVA_BORT+Jetour+Т2+2023-2024+black+12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JETOUR T2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EVA_BORT+Jetour+X70 plus+2020-2024+black+12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JETOUR X70 PLUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EVA_BORT+Jetour+X90 plus+2021-2024+black+12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JETOUR X90 PLUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EVA_BORT+Lada+_Niva+1977-2020+black+11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LADA NIVA 2121</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EVA_BORT+Volkswagen+Tiguan+2016-2021+black+12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOTOK+Ковер лоток+50х45++black+20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Коврик под лоток</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50*45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MISKA+Ковер миска+40х40++grey+9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40*40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOM80+Ковер 80х50+80х50++grey+11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Коврик придверный</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80*50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOM80+Ковер 80х50+80х50++grey+6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LODKA+Звезда+380++grey+11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Лодка Звезда 380</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LODKA+Звезда Тримаран 360+НДНД+grey+11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Лодка Звезда Тримаран 360</t>
+  </si>
+  <si>
+    <t xml:space="preserve">НУЖНО ЗАПИСАТЬ ВИДЕО</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LODKA+Навигатор 380R PRO+риб+grey+11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Лодка Навигатор 380R PRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LODKA+Нордик 360+пайол+grey+11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Лодка Нордик 360</t>
   </si>
 </sst>
 </file>
@@ -361,7 +508,7 @@
     <numFmt numFmtId="165" formatCode="[$-419]d\ mmm;@"/>
     <numFmt numFmtId="166" formatCode="d\-mmm"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -426,6 +573,13 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF070707"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -488,7 +642,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -538,6 +692,22 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -626,13 +796,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P227"/>
+  <dimension ref="A1:P265"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C227" activeCellId="0" sqref="C227"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A50" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R70" activeCellId="0" sqref="R70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.79296875" defaultRowHeight="51" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.80078125" defaultRowHeight="51" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="12.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="56.45"/>
@@ -2117,1697 +2287,2099 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="8" t="n">
-        <v>45876</v>
-      </c>
-      <c r="B40" s="8" t="n">
-        <v>45877</v>
-      </c>
-      <c r="C40" s="8"/>
+      <c r="A40" s="13" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B40" s="13" t="n">
+        <v>45904</v>
+      </c>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I40" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J40" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="K40" s="14" t="n">
+        <v>11</v>
+      </c>
+      <c r="L40" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="M40" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="N40" s="13"/>
     </row>
     <row r="41" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="8" t="n">
-        <v>45876</v>
-      </c>
-      <c r="B41" s="8" t="n">
-        <v>45877</v>
-      </c>
-      <c r="C41" s="8"/>
+      <c r="A41" s="13" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B41" s="13" t="n">
+        <v>45904</v>
+      </c>
+      <c r="C41" s="13"/>
+      <c r="D41" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K41" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="L41" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="M41" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="N41" s="4"/>
     </row>
     <row r="42" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="8" t="n">
-        <v>45876</v>
-      </c>
-      <c r="B42" s="8" t="n">
-        <v>45877</v>
-      </c>
-      <c r="C42" s="8"/>
+      <c r="A42" s="13" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B42" s="13" t="n">
+        <v>45904</v>
+      </c>
+      <c r="C42" s="13"/>
+      <c r="D42" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="E42" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I42" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J42" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K42" s="14" t="n">
+        <v>16</v>
+      </c>
+      <c r="L42" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="M42" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="N42" s="14" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="8" t="n">
-        <v>45875</v>
-      </c>
-      <c r="B43" s="8" t="n">
-        <v>45876</v>
-      </c>
-      <c r="C43" s="8"/>
+      <c r="A43" s="13" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B43" s="13" t="n">
+        <v>45904</v>
+      </c>
+      <c r="C43" s="13"/>
+      <c r="D43" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J43" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K43" s="14" t="n">
+        <v>11</v>
+      </c>
+      <c r="L43" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="M43" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="N43" s="4" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="8" t="n">
-        <v>45875</v>
-      </c>
-      <c r="B44" s="8" t="n">
-        <v>45876</v>
-      </c>
-      <c r="C44" s="8"/>
+      <c r="A44" s="13" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B44" s="13" t="n">
+        <v>45904</v>
+      </c>
+      <c r="C44" s="13"/>
+      <c r="D44" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K44" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="L44" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="M44" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="N44" s="4" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B45" s="8" t="n">
-        <v>45875</v>
-      </c>
-      <c r="C45" s="8"/>
+      <c r="A45" s="13" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B45" s="13" t="n">
+        <v>45904</v>
+      </c>
+      <c r="C45" s="13"/>
+      <c r="D45" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="E45" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="I45" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="J45" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="K45" s="15" t="n">
+        <v>12</v>
+      </c>
+      <c r="L45" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="M45" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="N45" s="15"/>
     </row>
     <row r="46" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B46" s="8" t="n">
-        <v>45875</v>
-      </c>
-      <c r="C46" s="8"/>
+      <c r="A46" s="13" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B46" s="13" t="n">
+        <v>45904</v>
+      </c>
+      <c r="C46" s="13"/>
+      <c r="D46" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="F46" s="14"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I46" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J46" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K46" s="14" t="n">
+        <v>12</v>
+      </c>
+      <c r="L46" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="M46" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="N46" s="14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B47" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="C47" s="8"/>
+      <c r="A47" s="13" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B47" s="13" t="n">
+        <v>45904</v>
+      </c>
+      <c r="C47" s="13"/>
+      <c r="D47" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="E47" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I47" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J47" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K47" s="14" t="n">
+        <v>12</v>
+      </c>
+      <c r="L47" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="M47" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="N47" s="14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="8" t="n">
-        <v>45871</v>
-      </c>
-      <c r="B48" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="C48" s="8"/>
+      <c r="A48" s="13" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B48" s="13" t="n">
+        <v>45904</v>
+      </c>
+      <c r="C48" s="13"/>
+      <c r="D48" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="E48" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I48" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J48" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K48" s="14" t="n">
+        <v>12</v>
+      </c>
+      <c r="L48" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="M48" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="N48" s="14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B49" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="C49" s="8"/>
+      <c r="A49" s="13" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B49" s="13" t="n">
+        <v>45904</v>
+      </c>
+      <c r="C49" s="13"/>
+      <c r="D49" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="E49" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="I49" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J49" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="K49" s="14" t="n">
+        <v>11</v>
+      </c>
+      <c r="L49" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="M49" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="N49" s="14" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="4" t="n">
-        <v>45879</v>
-      </c>
-      <c r="B50" s="4" t="n">
-        <v>45880</v>
-      </c>
-      <c r="C50" s="4"/>
+      <c r="A50" s="13" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B50" s="13" t="n">
+        <v>45904</v>
+      </c>
+      <c r="C50" s="13"/>
+      <c r="D50" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="E50" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I50" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J50" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="K50" s="14" t="n">
+        <v>10</v>
+      </c>
+      <c r="L50" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="M50" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="N50" s="14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="8" t="n">
-        <v>45878</v>
-      </c>
-      <c r="B51" s="8" t="n">
-        <v>45879</v>
-      </c>
-      <c r="C51" s="8"/>
+      <c r="A51" s="13" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B51" s="13" t="n">
+        <v>45904</v>
+      </c>
+      <c r="C51" s="13"/>
+      <c r="D51" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="E51" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I51" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J51" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="K51" s="14" t="n">
+        <v>11</v>
+      </c>
+      <c r="L51" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="M51" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="N51" s="14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="8" t="n">
-        <v>45877</v>
-      </c>
-      <c r="B52" s="8" t="n">
-        <v>45878</v>
-      </c>
-      <c r="C52" s="8"/>
+      <c r="A52" s="13" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B52" s="13" t="n">
+        <v>45904</v>
+      </c>
+      <c r="C52" s="13"/>
+      <c r="D52" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="E52" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I52" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J52" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K52" s="14" t="n">
+        <v>12</v>
+      </c>
+      <c r="L52" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="M52" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="N52" s="14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="8" t="n">
-        <v>45871</v>
-      </c>
-      <c r="B53" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="C53" s="8"/>
+      <c r="A53" s="13" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B53" s="13" t="n">
+        <v>45904</v>
+      </c>
+      <c r="C53" s="13"/>
+      <c r="D53" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="E53" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I53" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J53" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K53" s="14" t="n">
+        <v>12</v>
+      </c>
+      <c r="L53" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="M53" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="N53" s="14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="8" t="n">
-        <v>45877</v>
-      </c>
-      <c r="B54" s="8" t="n">
-        <v>45878</v>
-      </c>
-      <c r="C54" s="8"/>
+      <c r="A54" s="13" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B54" s="13" t="n">
+        <v>45904</v>
+      </c>
+      <c r="C54" s="13"/>
+      <c r="D54" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="E54" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="F54" s="14"/>
+      <c r="G54" s="14"/>
+      <c r="H54" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I54" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J54" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K54" s="14" t="n">
+        <v>12</v>
+      </c>
+      <c r="L54" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="M54" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="N54" s="14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B55" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="C55" s="8"/>
+      <c r="A55" s="13" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B55" s="13" t="n">
+        <v>45904</v>
+      </c>
+      <c r="C55" s="13"/>
+      <c r="D55" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="E55" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="F55" s="14"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I55" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J55" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K55" s="14" t="n">
+        <v>11</v>
+      </c>
+      <c r="L55" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="M55" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="N55" s="14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="8" t="n">
-        <v>45879</v>
-      </c>
-      <c r="B56" s="8" t="n">
-        <v>45880</v>
-      </c>
-      <c r="C56" s="8"/>
+      <c r="A56" s="13" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B56" s="13" t="n">
+        <v>45904</v>
+      </c>
+      <c r="C56" s="13"/>
+      <c r="D56" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E56" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F56" s="15"/>
+      <c r="G56" s="15"/>
+      <c r="H56" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="I56" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="J56" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="K56" s="15" t="n">
+        <v>12</v>
+      </c>
+      <c r="L56" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="M56" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="N56" s="15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="8" t="n">
-        <v>45878</v>
-      </c>
-      <c r="B57" s="8" t="n">
-        <v>45879</v>
-      </c>
-      <c r="C57" s="8"/>
+      <c r="A57" s="13" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B57" s="13" t="n">
+        <v>45904</v>
+      </c>
+      <c r="C57" s="13"/>
+      <c r="D57" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="E57" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F57" s="14"/>
+      <c r="G57" s="14"/>
+      <c r="H57" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I57" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J57" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K57" s="14" t="n">
+        <v>12</v>
+      </c>
+      <c r="L57" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="M57" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="N57" s="14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="4" t="n">
-        <v>45879</v>
-      </c>
-      <c r="B58" s="4" t="n">
-        <v>45880</v>
-      </c>
-      <c r="C58" s="4"/>
+      <c r="A58" s="13" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B58" s="13" t="n">
+        <v>45904</v>
+      </c>
+      <c r="C58" s="13"/>
+      <c r="D58" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="E58" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F58" s="14"/>
+      <c r="G58" s="14"/>
+      <c r="H58" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="I58" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="J58" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K58" s="14" t="n">
+        <v>11</v>
+      </c>
+      <c r="L58" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M58" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N58" s="14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="4" t="n">
-        <v>45879</v>
-      </c>
-      <c r="B59" s="4" t="n">
-        <v>45880</v>
-      </c>
-      <c r="C59" s="4"/>
+      <c r="A59" s="13" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B59" s="13" t="n">
+        <v>45904</v>
+      </c>
+      <c r="C59" s="13"/>
+      <c r="D59" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E59" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="F59" s="14"/>
+      <c r="G59" s="14"/>
+      <c r="H59" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="I59" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J59" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="K59" s="14" t="n">
+        <v>11</v>
+      </c>
+      <c r="L59" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M59" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N59" s="14" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="8" t="n">
-        <v>45870</v>
-      </c>
-      <c r="B60" s="8" t="n">
-        <v>45871</v>
-      </c>
-      <c r="C60" s="8"/>
+      <c r="A60" s="13" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B60" s="13" t="n">
+        <v>45904</v>
+      </c>
+      <c r="C60" s="13"/>
+      <c r="D60" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E60" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="F60" s="15"/>
+      <c r="G60" s="15"/>
+      <c r="H60" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="I60" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="J60" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="K60" s="15" t="n">
+        <v>12</v>
+      </c>
+      <c r="L60" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M60" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N60" s="15" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="13" t="n">
-        <v>45869</v>
+        <v>45903</v>
       </c>
       <c r="B61" s="13" t="n">
-        <v>45870</v>
+        <v>45904</v>
       </c>
       <c r="C61" s="13"/>
+      <c r="D61" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="E61" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="F61" s="14"/>
+      <c r="G61" s="14"/>
+      <c r="H61" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="I61" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J61" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K61" s="14" t="n">
+        <v>20</v>
+      </c>
+      <c r="L61" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M61" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N61" s="14" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="8" t="n">
-        <v>45878</v>
-      </c>
-      <c r="B62" s="8" t="n">
-        <v>45879</v>
-      </c>
-      <c r="C62" s="8"/>
+      <c r="A62" s="13" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B62" s="13" t="n">
+        <v>45904</v>
+      </c>
+      <c r="C62" s="13"/>
+      <c r="D62" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E62" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="F62" s="14"/>
+      <c r="G62" s="14"/>
+      <c r="H62" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="I62" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J62" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K62" s="14" t="n">
+        <v>13</v>
+      </c>
+      <c r="L62" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M62" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N62" s="14" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="4" t="n">
-        <v>45880</v>
-      </c>
-      <c r="B63" s="4" t="n">
-        <v>45881</v>
-      </c>
-      <c r="C63" s="4"/>
+      <c r="A63" s="13" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B63" s="13" t="n">
+        <v>45904</v>
+      </c>
+      <c r="C63" s="13"/>
+      <c r="D63" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="E63" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="F63" s="14"/>
+      <c r="G63" s="14"/>
+      <c r="H63" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="I63" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="J63" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K63" s="14" t="n">
+        <v>8</v>
+      </c>
+      <c r="L63" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M63" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N63" s="14" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B64" s="8" t="n">
-        <v>45875</v>
-      </c>
-      <c r="C64" s="8"/>
+      <c r="A64" s="13" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B64" s="13" t="n">
+        <v>45904</v>
+      </c>
+      <c r="C64" s="13"/>
+      <c r="D64" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="E64" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="F64" s="14"/>
+      <c r="G64" s="14"/>
+      <c r="H64" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="I64" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="J64" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K64" s="14" t="n">
+        <v>11</v>
+      </c>
+      <c r="L64" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M64" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N64" s="14" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="8" t="n">
-        <v>45870</v>
-      </c>
-      <c r="B65" s="8" t="n">
-        <v>45871</v>
-      </c>
-      <c r="C65" s="8"/>
+      <c r="A65" s="13" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B65" s="13" t="n">
+        <v>45904</v>
+      </c>
+      <c r="C65" s="13"/>
+      <c r="D65" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="E65" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="F65" s="14"/>
+      <c r="G65" s="14"/>
+      <c r="H65" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="I65" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="J65" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K65" s="14" t="n">
+        <v>6</v>
+      </c>
+      <c r="L65" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M65" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N65" s="14" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="8" t="n">
-        <v>45870</v>
-      </c>
-      <c r="B66" s="8" t="n">
-        <v>45871</v>
-      </c>
-      <c r="C66" s="8"/>
+      <c r="A66" s="13" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B66" s="13" t="n">
+        <v>45904</v>
+      </c>
+      <c r="C66" s="13"/>
+      <c r="D66" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="E66" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="F66" s="15"/>
+      <c r="G66" s="15"/>
+      <c r="H66" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="I66" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="J66" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="K66" s="15" t="n">
+        <v>11</v>
+      </c>
+      <c r="L66" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M66" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N66" s="15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="8" t="n">
-        <v>45878</v>
-      </c>
-      <c r="B67" s="8" t="n">
-        <v>45880</v>
-      </c>
-      <c r="C67" s="8"/>
+      <c r="A67" s="13" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B67" s="13" t="n">
+        <v>45904</v>
+      </c>
+      <c r="C67" s="13"/>
+      <c r="D67" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="E67" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="F67" s="15"/>
+      <c r="G67" s="15"/>
+      <c r="H67" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="I67" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="J67" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="K67" s="15" t="n">
+        <v>11</v>
+      </c>
+      <c r="L67" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M67" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N67" s="15" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B68" s="8" t="n">
-        <v>45877</v>
-      </c>
-      <c r="C68" s="8"/>
+      <c r="A68" s="13" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B68" s="13" t="n">
+        <v>45904</v>
+      </c>
+      <c r="C68" s="13"/>
+      <c r="D68" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="E68" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="F68" s="15"/>
+      <c r="G68" s="15"/>
+      <c r="H68" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="I68" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="J68" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="K68" s="15" t="n">
+        <v>11</v>
+      </c>
+      <c r="L68" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M68" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N68" s="15" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="13" t="n">
-        <v>45869</v>
+        <v>45903</v>
       </c>
       <c r="B69" s="13" t="n">
-        <v>45870</v>
+        <v>45904</v>
       </c>
       <c r="C69" s="13"/>
+      <c r="D69" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="E69" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="F69" s="15"/>
+      <c r="G69" s="15"/>
+      <c r="H69" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="I69" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="J69" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="K69" s="15" t="n">
+        <v>11</v>
+      </c>
+      <c r="L69" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M69" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N69" s="15" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B70" s="8" t="n">
-        <v>45875</v>
-      </c>
-      <c r="C70" s="8"/>
+      <c r="A70" s="13" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B70" s="13" t="n">
+        <v>45904</v>
+      </c>
+      <c r="C70" s="13"/>
+      <c r="D70" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E70" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="F70" s="14"/>
+      <c r="G70" s="14"/>
+      <c r="H70" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="I70" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="J70" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K70" s="14" t="n">
+        <v>11</v>
+      </c>
+      <c r="L70" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M70" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N70" s="14" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="8" t="n">
-        <v>45871</v>
-      </c>
-      <c r="B71" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="C71" s="8"/>
+      <c r="A71" s="13" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B71" s="13" t="n">
+        <v>45904</v>
+      </c>
+      <c r="C71" s="13"/>
+      <c r="D71" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="E71" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="F71" s="14"/>
+      <c r="G71" s="14"/>
+      <c r="H71" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="I71" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="J71" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K71" s="14" t="n">
+        <v>11</v>
+      </c>
+      <c r="L71" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M71" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N71" s="14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="8" t="n">
-        <v>45871</v>
-      </c>
-      <c r="B72" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="C72" s="8"/>
+      <c r="A72" s="13" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B72" s="13" t="n">
+        <v>45904</v>
+      </c>
+      <c r="C72" s="13"/>
+      <c r="D72" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="E72" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="F72" s="14"/>
+      <c r="G72" s="14"/>
+      <c r="H72" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="I72" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="J72" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K72" s="14" t="n">
+        <v>11</v>
+      </c>
+      <c r="L72" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M72" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N72" s="14" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="4" t="n">
-        <v>45880</v>
-      </c>
-      <c r="B73" s="4" t="n">
-        <v>45881</v>
-      </c>
-      <c r="C73" s="4"/>
+      <c r="A73" s="13" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B73" s="13" t="n">
+        <v>45904</v>
+      </c>
+      <c r="C73" s="13"/>
+      <c r="D73" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="E73" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F73" s="14"/>
+      <c r="G73" s="14"/>
+      <c r="H73" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="I73" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="J73" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K73" s="14" t="n">
+        <v>11</v>
+      </c>
+      <c r="L73" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M73" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N73" s="14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="4" t="n">
-        <v>45879</v>
-      </c>
-      <c r="B74" s="4" t="n">
-        <v>45880</v>
-      </c>
+      <c r="A74" s="4"/>
+      <c r="B74" s="4"/>
       <c r="C74" s="4"/>
     </row>
     <row r="75" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="4" t="n">
-        <v>45879</v>
-      </c>
-      <c r="B75" s="4" t="n">
-        <v>45880</v>
-      </c>
+      <c r="A75" s="4"/>
+      <c r="B75" s="4"/>
       <c r="C75" s="4"/>
     </row>
     <row r="76" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="8" t="n">
-        <v>45876</v>
-      </c>
-      <c r="B76" s="8" t="n">
-        <v>45877</v>
-      </c>
+      <c r="A76" s="8"/>
+      <c r="B76" s="8"/>
       <c r="C76" s="8"/>
     </row>
     <row r="77" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="8" t="n">
-        <v>45875</v>
-      </c>
-      <c r="B77" s="8" t="n">
-        <v>45876</v>
-      </c>
+      <c r="A77" s="8"/>
+      <c r="B77" s="8"/>
       <c r="C77" s="8"/>
     </row>
     <row r="78" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B78" s="8" t="n">
-        <v>45875</v>
-      </c>
+      <c r="A78" s="8"/>
+      <c r="B78" s="8"/>
       <c r="C78" s="8"/>
     </row>
     <row r="79" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B79" s="8" t="n">
-        <v>45875</v>
-      </c>
+      <c r="A79" s="8"/>
+      <c r="B79" s="8"/>
       <c r="C79" s="8"/>
     </row>
     <row r="80" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B80" s="8" t="n">
-        <v>45874</v>
-      </c>
+      <c r="A80" s="8"/>
+      <c r="B80" s="8"/>
       <c r="C80" s="8"/>
     </row>
     <row r="81" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B81" s="8" t="n">
-        <v>45873</v>
-      </c>
+      <c r="A81" s="8"/>
+      <c r="B81" s="8"/>
       <c r="C81" s="8"/>
     </row>
     <row r="82" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B82" s="8" t="n">
-        <v>45873</v>
-      </c>
+      <c r="A82" s="8"/>
+      <c r="B82" s="8"/>
       <c r="C82" s="8"/>
     </row>
     <row r="83" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A83" s="8" t="n">
-        <v>45871</v>
-      </c>
-      <c r="B83" s="8" t="n">
-        <v>45872</v>
-      </c>
+      <c r="A83" s="8"/>
+      <c r="B83" s="8"/>
       <c r="C83" s="8"/>
     </row>
     <row r="84" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A84" s="8" t="n">
-        <v>45870</v>
-      </c>
-      <c r="B84" s="8" t="n">
-        <v>45871</v>
-      </c>
+      <c r="A84" s="8"/>
+      <c r="B84" s="8"/>
       <c r="C84" s="8"/>
     </row>
     <row r="85" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A85" s="8" t="n">
-        <v>45870</v>
-      </c>
-      <c r="B85" s="8" t="n">
-        <v>45871</v>
-      </c>
+      <c r="A85" s="8"/>
+      <c r="B85" s="8"/>
       <c r="C85" s="8"/>
     </row>
     <row r="86" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A86" s="8" t="n">
-        <v>45871</v>
-      </c>
-      <c r="B86" s="8" t="n">
-        <v>45872</v>
-      </c>
+      <c r="A86" s="8"/>
+      <c r="B86" s="8"/>
       <c r="C86" s="8"/>
     </row>
     <row r="87" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A87" s="8" t="n">
-        <v>45875</v>
-      </c>
-      <c r="B87" s="8" t="n">
-        <v>45876</v>
-      </c>
+      <c r="A87" s="8"/>
+      <c r="B87" s="8"/>
       <c r="C87" s="8"/>
     </row>
     <row r="88" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A88" s="8" t="n">
-        <v>45870</v>
-      </c>
-      <c r="B88" s="8" t="n">
-        <v>45871</v>
-      </c>
+      <c r="A88" s="8"/>
+      <c r="B88" s="8"/>
       <c r="C88" s="8"/>
     </row>
     <row r="89" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A89" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B89" s="8" t="n">
-        <v>45872</v>
-      </c>
+      <c r="A89" s="8"/>
+      <c r="B89" s="8"/>
       <c r="C89" s="8"/>
     </row>
     <row r="90" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A90" s="8" t="n">
-        <v>45878</v>
-      </c>
-      <c r="B90" s="8" t="n">
-        <v>45879</v>
-      </c>
+      <c r="A90" s="8"/>
+      <c r="B90" s="8"/>
       <c r="C90" s="8"/>
     </row>
     <row r="91" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A91" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B91" s="8" t="n">
-        <v>45875</v>
-      </c>
+      <c r="A91" s="8"/>
+      <c r="B91" s="8"/>
       <c r="C91" s="8"/>
     </row>
     <row r="92" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A92" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B92" s="8" t="n">
-        <v>45875</v>
-      </c>
+      <c r="A92" s="8"/>
+      <c r="B92" s="8"/>
       <c r="C92" s="8"/>
     </row>
     <row r="93" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A93" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B93" s="8" t="n">
-        <v>45874</v>
-      </c>
+      <c r="A93" s="8"/>
+      <c r="B93" s="8"/>
       <c r="C93" s="8"/>
     </row>
     <row r="94" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A94" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B94" s="8" t="n">
-        <v>45873</v>
-      </c>
+      <c r="A94" s="8"/>
+      <c r="B94" s="8"/>
       <c r="C94" s="8"/>
     </row>
     <row r="95" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A95" s="8" t="n">
-        <v>45871</v>
-      </c>
-      <c r="B95" s="8" t="n">
-        <v>45872</v>
-      </c>
+      <c r="A95" s="8"/>
+      <c r="B95" s="8"/>
       <c r="C95" s="8"/>
     </row>
     <row r="96" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A96" s="8" t="n">
-        <v>45877</v>
-      </c>
-      <c r="B96" s="8" t="n">
-        <v>45878</v>
-      </c>
+      <c r="A96" s="8"/>
+      <c r="B96" s="8"/>
       <c r="C96" s="8"/>
     </row>
     <row r="97" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A97" s="8" t="n">
-        <v>45877</v>
-      </c>
-      <c r="B97" s="8" t="n">
-        <v>45878</v>
-      </c>
+      <c r="A97" s="8"/>
+      <c r="B97" s="8"/>
       <c r="C97" s="8"/>
     </row>
     <row r="98" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A98" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B98" s="8" t="n">
-        <v>45875</v>
-      </c>
+      <c r="A98" s="8"/>
+      <c r="B98" s="8"/>
       <c r="C98" s="8"/>
     </row>
     <row r="99" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A99" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B99" s="8" t="n">
-        <v>45873</v>
-      </c>
+      <c r="A99" s="8"/>
+      <c r="B99" s="8"/>
       <c r="C99" s="8"/>
     </row>
     <row r="100" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A100" s="8" t="n">
-        <v>45871</v>
-      </c>
-      <c r="B100" s="8" t="n">
-        <v>45872</v>
-      </c>
+      <c r="A100" s="8"/>
+      <c r="B100" s="8"/>
       <c r="C100" s="8"/>
     </row>
     <row r="101" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A101" s="4" t="n">
-        <v>45879</v>
-      </c>
-      <c r="B101" s="4" t="n">
-        <v>45880</v>
-      </c>
+      <c r="A101" s="4"/>
+      <c r="B101" s="4"/>
       <c r="C101" s="4"/>
     </row>
     <row r="102" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A102" s="8" t="n">
-        <v>45878</v>
-      </c>
-      <c r="B102" s="8" t="n">
-        <v>45878</v>
-      </c>
+      <c r="A102" s="8"/>
+      <c r="B102" s="8"/>
       <c r="C102" s="8"/>
     </row>
     <row r="103" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A103" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B103" s="8" t="n">
-        <v>45875</v>
-      </c>
+      <c r="A103" s="8"/>
+      <c r="B103" s="8"/>
       <c r="C103" s="8"/>
     </row>
     <row r="104" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A104" s="8" t="n">
-        <v>45877</v>
-      </c>
-      <c r="B104" s="8" t="n">
-        <v>45878</v>
-      </c>
+      <c r="A104" s="8"/>
+      <c r="B104" s="8"/>
       <c r="C104" s="8"/>
     </row>
     <row r="105" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A105" s="8" t="n">
-        <v>45870</v>
-      </c>
-      <c r="B105" s="8" t="n">
-        <v>45871</v>
-      </c>
+      <c r="A105" s="8"/>
+      <c r="B105" s="8"/>
       <c r="C105" s="8"/>
     </row>
     <row r="106" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A106" s="8" t="n">
-        <v>45876</v>
-      </c>
-      <c r="B106" s="8" t="n">
-        <v>45877</v>
-      </c>
+      <c r="A106" s="8"/>
+      <c r="B106" s="8"/>
       <c r="C106" s="8"/>
     </row>
     <row r="107" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A107" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B107" s="8" t="n">
-        <v>45874</v>
-      </c>
+      <c r="A107" s="8"/>
+      <c r="B107" s="8"/>
       <c r="C107" s="8"/>
     </row>
     <row r="108" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A108" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B108" s="8" t="n">
-        <v>45874</v>
-      </c>
+      <c r="A108" s="8"/>
+      <c r="B108" s="8"/>
       <c r="C108" s="8"/>
     </row>
     <row r="109" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A109" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B109" s="8" t="n">
-        <v>45873</v>
-      </c>
+      <c r="A109" s="8"/>
+      <c r="B109" s="8"/>
       <c r="C109" s="8"/>
     </row>
     <row r="110" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A110" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B110" s="8" t="n">
-        <v>45873</v>
-      </c>
+      <c r="A110" s="8"/>
+      <c r="B110" s="8"/>
       <c r="C110" s="8"/>
     </row>
     <row r="111" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A111" s="4" t="n">
-        <v>45879</v>
-      </c>
-      <c r="B111" s="4" t="n">
-        <v>45880</v>
-      </c>
+      <c r="A111" s="4"/>
+      <c r="B111" s="4"/>
       <c r="C111" s="4"/>
     </row>
     <row r="112" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A112" s="8" t="n">
-        <v>45878</v>
-      </c>
-      <c r="B112" s="8" t="n">
-        <v>45879</v>
-      </c>
+      <c r="A112" s="8"/>
+      <c r="B112" s="8"/>
       <c r="C112" s="8"/>
     </row>
     <row r="113" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A113" s="8" t="n">
-        <v>45878</v>
-      </c>
-      <c r="B113" s="8" t="n">
-        <v>45879</v>
-      </c>
+      <c r="A113" s="8"/>
+      <c r="B113" s="8"/>
       <c r="C113" s="8"/>
     </row>
     <row r="114" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A114" s="8" t="n">
-        <v>45876</v>
-      </c>
-      <c r="B114" s="8" t="n">
-        <v>45877</v>
-      </c>
+      <c r="A114" s="8"/>
+      <c r="B114" s="8"/>
       <c r="C114" s="8"/>
     </row>
     <row r="115" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A115" s="8" t="n">
-        <v>45875</v>
-      </c>
-      <c r="B115" s="8" t="n">
-        <v>45876</v>
-      </c>
+      <c r="A115" s="8"/>
+      <c r="B115" s="8"/>
       <c r="C115" s="8"/>
     </row>
     <row r="116" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A116" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B116" s="8" t="n">
-        <v>45875</v>
-      </c>
+      <c r="A116" s="8"/>
+      <c r="B116" s="8"/>
       <c r="C116" s="8"/>
     </row>
     <row r="117" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A117" s="8" t="n">
-        <v>45870</v>
-      </c>
-      <c r="B117" s="8" t="n">
-        <v>45871</v>
-      </c>
+      <c r="A117" s="8"/>
+      <c r="B117" s="8"/>
       <c r="C117" s="8"/>
     </row>
     <row r="118" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A118" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B118" s="8" t="n">
-        <v>45874</v>
-      </c>
+      <c r="A118" s="8"/>
+      <c r="B118" s="8"/>
       <c r="C118" s="8"/>
     </row>
     <row r="119" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A119" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B119" s="8" t="n">
-        <v>45872</v>
-      </c>
+      <c r="A119" s="8"/>
+      <c r="B119" s="8"/>
       <c r="C119" s="8"/>
     </row>
     <row r="120" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A120" s="13" t="n">
-        <v>45869</v>
-      </c>
-      <c r="B120" s="13" t="n">
-        <v>45870</v>
-      </c>
-      <c r="C120" s="13"/>
+      <c r="A120" s="17"/>
+      <c r="B120" s="17"/>
+      <c r="C120" s="17"/>
     </row>
     <row r="121" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A121" s="8" t="n">
-        <v>45876</v>
-      </c>
-      <c r="B121" s="8" t="n">
-        <v>45877</v>
-      </c>
+      <c r="A121" s="8"/>
+      <c r="B121" s="8"/>
       <c r="C121" s="8"/>
     </row>
     <row r="122" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A122" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B122" s="8" t="n">
-        <v>45874</v>
-      </c>
+      <c r="A122" s="8"/>
+      <c r="B122" s="8"/>
       <c r="C122" s="8"/>
     </row>
     <row r="123" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A123" s="8" t="n">
-        <v>45878</v>
-      </c>
-      <c r="B123" s="8" t="n">
-        <v>45878</v>
-      </c>
+      <c r="A123" s="8"/>
+      <c r="B123" s="8"/>
       <c r="C123" s="8"/>
     </row>
     <row r="124" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A124" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B124" s="8" t="n">
-        <v>45873</v>
-      </c>
+      <c r="A124" s="8"/>
+      <c r="B124" s="8"/>
       <c r="C124" s="8"/>
     </row>
     <row r="125" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A125" s="4" t="n">
-        <v>45880</v>
-      </c>
-      <c r="B125" s="4" t="n">
-        <v>45881</v>
-      </c>
+      <c r="A125" s="4"/>
+      <c r="B125" s="4"/>
       <c r="C125" s="4"/>
     </row>
     <row r="126" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A126" s="8" t="n">
-        <v>45879</v>
-      </c>
-      <c r="B126" s="8" t="n">
-        <v>45880</v>
-      </c>
+      <c r="A126" s="8"/>
+      <c r="B126" s="8"/>
       <c r="C126" s="8"/>
     </row>
     <row r="127" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A127" s="8" t="n">
-        <v>45879</v>
-      </c>
-      <c r="B127" s="8" t="n">
-        <v>45880</v>
-      </c>
+      <c r="A127" s="8"/>
+      <c r="B127" s="8"/>
       <c r="C127" s="8"/>
     </row>
     <row r="128" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A128" s="8" t="n">
-        <v>45878</v>
-      </c>
-      <c r="B128" s="8" t="n">
-        <v>45879</v>
-      </c>
+      <c r="A128" s="8"/>
+      <c r="B128" s="8"/>
       <c r="C128" s="8"/>
     </row>
     <row r="129" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A129" s="8" t="n">
-        <v>45878</v>
-      </c>
-      <c r="B129" s="8" t="n">
-        <v>45879</v>
-      </c>
+      <c r="A129" s="8"/>
+      <c r="B129" s="8"/>
       <c r="C129" s="8"/>
     </row>
     <row r="130" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A130" s="8" t="n">
-        <v>45877</v>
-      </c>
-      <c r="B130" s="8" t="n">
-        <v>45878</v>
-      </c>
+      <c r="A130" s="8"/>
+      <c r="B130" s="8"/>
       <c r="C130" s="8"/>
     </row>
     <row r="131" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A131" s="8" t="n">
-        <v>45875</v>
-      </c>
-      <c r="B131" s="8" t="n">
-        <v>45876</v>
-      </c>
+      <c r="A131" s="8"/>
+      <c r="B131" s="8"/>
       <c r="C131" s="8"/>
     </row>
     <row r="132" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A132" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B132" s="8" t="n">
-        <v>45875</v>
-      </c>
+      <c r="A132" s="8"/>
+      <c r="B132" s="8"/>
       <c r="C132" s="8"/>
     </row>
     <row r="133" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A133" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B133" s="8" t="n">
-        <v>45875</v>
-      </c>
+      <c r="A133" s="8"/>
+      <c r="B133" s="8"/>
       <c r="C133" s="8"/>
     </row>
     <row r="134" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A134" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B134" s="8" t="n">
-        <v>45874</v>
-      </c>
+      <c r="A134" s="8"/>
+      <c r="B134" s="8"/>
       <c r="C134" s="8"/>
     </row>
     <row r="135" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A135" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B135" s="8" t="n">
-        <v>45873</v>
-      </c>
+      <c r="A135" s="8"/>
+      <c r="B135" s="8"/>
       <c r="C135" s="8"/>
     </row>
     <row r="136" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A136" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B136" s="8" t="n">
-        <v>45873</v>
-      </c>
+      <c r="A136" s="8"/>
+      <c r="B136" s="8"/>
       <c r="C136" s="8"/>
     </row>
     <row r="137" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A137" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B137" s="8" t="n">
-        <v>45873</v>
-      </c>
+      <c r="A137" s="8"/>
+      <c r="B137" s="8"/>
       <c r="C137" s="8"/>
     </row>
     <row r="138" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A138" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B138" s="8" t="n">
-        <v>45873</v>
-      </c>
+      <c r="A138" s="8"/>
+      <c r="B138" s="8"/>
       <c r="C138" s="8"/>
     </row>
     <row r="139" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A139" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B139" s="8" t="n">
-        <v>45873</v>
-      </c>
+      <c r="A139" s="8"/>
+      <c r="B139" s="8"/>
       <c r="C139" s="8"/>
     </row>
     <row r="140" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A140" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B140" s="8" t="n">
-        <v>45873</v>
-      </c>
+      <c r="A140" s="8"/>
+      <c r="B140" s="8"/>
       <c r="C140" s="8"/>
     </row>
     <row r="141" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A141" s="8" t="n">
-        <v>45871</v>
-      </c>
-      <c r="B141" s="8" t="n">
-        <v>45872</v>
-      </c>
+      <c r="A141" s="8"/>
+      <c r="B141" s="8"/>
       <c r="C141" s="8"/>
     </row>
     <row r="142" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A142" s="8" t="n">
-        <v>45871</v>
-      </c>
-      <c r="B142" s="8" t="n">
-        <v>45872</v>
-      </c>
+      <c r="A142" s="8"/>
+      <c r="B142" s="8"/>
       <c r="C142" s="8"/>
     </row>
     <row r="143" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A143" s="8" t="n">
-        <v>45871</v>
-      </c>
-      <c r="B143" s="8" t="n">
-        <v>45872</v>
-      </c>
+      <c r="A143" s="8"/>
+      <c r="B143" s="8"/>
       <c r="C143" s="8"/>
     </row>
     <row r="144" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A144" s="8" t="n">
-        <v>45871</v>
-      </c>
-      <c r="B144" s="8" t="n">
-        <v>45872</v>
-      </c>
+      <c r="A144" s="8"/>
+      <c r="B144" s="8"/>
       <c r="C144" s="8"/>
     </row>
     <row r="145" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A145" s="8" t="n">
-        <v>45878</v>
-      </c>
-      <c r="B145" s="8" t="n">
-        <v>45879</v>
-      </c>
+      <c r="A145" s="8"/>
+      <c r="B145" s="8"/>
       <c r="C145" s="8"/>
     </row>
     <row r="146" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A146" s="8" t="n">
-        <v>45877</v>
-      </c>
-      <c r="B146" s="8" t="n">
-        <v>45877</v>
-      </c>
+      <c r="A146" s="8"/>
+      <c r="B146" s="8"/>
       <c r="C146" s="8"/>
     </row>
     <row r="147" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A147" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B147" s="8" t="n">
-        <v>45874</v>
-      </c>
+      <c r="A147" s="8"/>
+      <c r="B147" s="8"/>
       <c r="C147" s="8"/>
     </row>
     <row r="148" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A148" s="8" t="n">
-        <v>45870</v>
-      </c>
-      <c r="B148" s="8" t="n">
-        <v>45871</v>
-      </c>
+      <c r="A148" s="8"/>
+      <c r="B148" s="8"/>
       <c r="C148" s="8"/>
     </row>
     <row r="149" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A149" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B149" s="8" t="n">
-        <v>45872</v>
-      </c>
+      <c r="A149" s="8"/>
+      <c r="B149" s="8"/>
       <c r="C149" s="8"/>
     </row>
     <row r="150" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A150" s="8" t="n">
-        <v>45871</v>
-      </c>
-      <c r="B150" s="8" t="n">
-        <v>45872</v>
-      </c>
+      <c r="A150" s="8"/>
+      <c r="B150" s="8"/>
       <c r="C150" s="8"/>
     </row>
     <row r="151" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A151" s="8" t="n">
-        <v>45870</v>
-      </c>
-      <c r="B151" s="8" t="n">
-        <v>45871</v>
-      </c>
+      <c r="A151" s="8"/>
+      <c r="B151" s="8"/>
       <c r="C151" s="8"/>
     </row>
     <row r="152" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A152" s="8" t="n">
-        <v>45870</v>
-      </c>
-      <c r="B152" s="8" t="n">
-        <v>45870</v>
-      </c>
+      <c r="A152" s="8"/>
+      <c r="B152" s="8"/>
       <c r="C152" s="8"/>
     </row>
     <row r="153" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A153" s="8" t="n">
-        <v>45877</v>
-      </c>
-      <c r="B153" s="8" t="n">
-        <v>45878</v>
-      </c>
+      <c r="A153" s="8"/>
+      <c r="B153" s="8"/>
       <c r="C153" s="8"/>
     </row>
     <row r="154" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A154" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B154" s="8" t="n">
-        <v>45873</v>
-      </c>
+      <c r="A154" s="8"/>
+      <c r="B154" s="8"/>
       <c r="C154" s="8"/>
     </row>
     <row r="155" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A155" s="13" t="n">
-        <v>45869</v>
-      </c>
-      <c r="B155" s="13" t="n">
-        <v>45870</v>
-      </c>
-      <c r="C155" s="13"/>
+      <c r="A155" s="17"/>
+      <c r="B155" s="17"/>
+      <c r="C155" s="17"/>
     </row>
     <row r="156" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A156" s="13" t="n">
-        <v>45869</v>
-      </c>
-      <c r="B156" s="13" t="n">
-        <v>45870</v>
-      </c>
-      <c r="C156" s="13"/>
+      <c r="A156" s="17"/>
+      <c r="B156" s="17"/>
+      <c r="C156" s="17"/>
     </row>
     <row r="157" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A157" s="13" t="n">
-        <v>45868</v>
-      </c>
-      <c r="B157" s="13" t="n">
-        <v>45870</v>
-      </c>
-      <c r="C157" s="13"/>
+      <c r="A157" s="17"/>
+      <c r="B157" s="17"/>
+      <c r="C157" s="17"/>
     </row>
     <row r="158" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A158" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B158" s="8" t="n">
-        <v>45873</v>
-      </c>
+      <c r="A158" s="8"/>
+      <c r="B158" s="8"/>
       <c r="C158" s="8"/>
     </row>
     <row r="159" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A159" s="8" t="n">
-        <v>45875</v>
-      </c>
-      <c r="B159" s="8" t="n">
-        <v>45876</v>
-      </c>
+      <c r="A159" s="8"/>
+      <c r="B159" s="8"/>
       <c r="C159" s="8"/>
     </row>
     <row r="160" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A160" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B160" s="8" t="n">
-        <v>45873</v>
-      </c>
+      <c r="A160" s="8"/>
+      <c r="B160" s="8"/>
       <c r="C160" s="8"/>
     </row>
     <row r="161" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A161" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B161" s="8" t="n">
-        <v>45873</v>
-      </c>
+      <c r="A161" s="8"/>
+      <c r="B161" s="8"/>
       <c r="C161" s="8"/>
     </row>
     <row r="162" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A162" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B162" s="8" t="n">
-        <v>45873</v>
-      </c>
+      <c r="A162" s="8"/>
+      <c r="B162" s="8"/>
       <c r="C162" s="8"/>
     </row>
     <row r="163" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A163" s="13" t="n">
-        <v>45869</v>
-      </c>
-      <c r="B163" s="13" t="n">
-        <v>45870</v>
-      </c>
-      <c r="C163" s="13"/>
+      <c r="A163" s="17"/>
+      <c r="B163" s="17"/>
+      <c r="C163" s="17"/>
     </row>
     <row r="164" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A164" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B164" s="8" t="n">
-        <v>45875</v>
-      </c>
+      <c r="A164" s="8"/>
+      <c r="B164" s="8"/>
       <c r="C164" s="8"/>
     </row>
     <row r="165" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A165" s="8" t="n">
-        <v>45875</v>
-      </c>
-      <c r="B165" s="8" t="n">
-        <v>45876</v>
-      </c>
+      <c r="A165" s="8"/>
+      <c r="B165" s="8"/>
       <c r="C165" s="8"/>
     </row>
     <row r="166" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A166" s="8" t="n">
-        <v>45871</v>
-      </c>
-      <c r="B166" s="8" t="n">
-        <v>45873</v>
-      </c>
+      <c r="A166" s="8"/>
+      <c r="B166" s="8"/>
       <c r="C166" s="8"/>
     </row>
     <row r="167" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A167" s="8" t="n">
-        <v>45877</v>
-      </c>
-      <c r="B167" s="8" t="n">
-        <v>45878</v>
-      </c>
+      <c r="A167" s="8"/>
+      <c r="B167" s="8"/>
       <c r="C167" s="8"/>
     </row>
     <row r="168" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A168" s="8" t="n">
-        <v>45877</v>
-      </c>
-      <c r="B168" s="8" t="n">
-        <v>45878</v>
-      </c>
+      <c r="A168" s="8"/>
+      <c r="B168" s="8"/>
       <c r="C168" s="8"/>
     </row>
     <row r="169" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A169" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B169" s="8" t="n">
-        <v>45873</v>
-      </c>
+      <c r="A169" s="8"/>
+      <c r="B169" s="8"/>
       <c r="C169" s="8"/>
     </row>
     <row r="170" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A170" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B170" s="8" t="n">
-        <v>45873</v>
-      </c>
+      <c r="A170" s="8"/>
+      <c r="B170" s="8"/>
       <c r="C170" s="8"/>
     </row>
     <row r="171" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A171" s="8" t="n">
-        <v>45870</v>
-      </c>
-      <c r="B171" s="8" t="n">
-        <v>45870</v>
-      </c>
+      <c r="A171" s="8"/>
+      <c r="B171" s="8"/>
       <c r="C171" s="8"/>
     </row>
     <row r="172" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A172" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B172" s="8" t="n">
-        <v>45874</v>
-      </c>
+      <c r="A172" s="8"/>
+      <c r="B172" s="8"/>
       <c r="C172" s="8"/>
     </row>
     <row r="173" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A173" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B173" s="8" t="n">
-        <v>45873</v>
-      </c>
+      <c r="A173" s="8"/>
+      <c r="B173" s="8"/>
       <c r="C173" s="8"/>
     </row>
     <row r="174" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A174" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B174" s="8" t="n">
-        <v>45873</v>
-      </c>
+      <c r="A174" s="8"/>
+      <c r="B174" s="8"/>
       <c r="C174" s="8"/>
     </row>
     <row r="175" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A175" s="8" t="n">
-        <v>45875</v>
-      </c>
-      <c r="B175" s="8" t="n">
-        <v>45876</v>
-      </c>
+      <c r="A175" s="8"/>
+      <c r="B175" s="8"/>
       <c r="C175" s="8"/>
     </row>
     <row r="176" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A176" s="8" t="n">
-        <v>45877</v>
-      </c>
-      <c r="B176" s="8" t="n">
-        <v>45878</v>
-      </c>
+      <c r="A176" s="8"/>
+      <c r="B176" s="8"/>
       <c r="C176" s="8"/>
     </row>
     <row r="177" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A177" s="8" t="n">
-        <v>45877</v>
-      </c>
-      <c r="B177" s="8" t="n">
-        <v>45877</v>
-      </c>
+      <c r="A177" s="8"/>
+      <c r="B177" s="8"/>
       <c r="C177" s="8"/>
     </row>
     <row r="178" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A178" s="8" t="n">
-        <v>45876</v>
-      </c>
-      <c r="B178" s="8" t="n">
-        <v>45877</v>
-      </c>
+      <c r="A178" s="8"/>
+      <c r="B178" s="8"/>
       <c r="C178" s="8"/>
     </row>
     <row r="179" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A179" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B179" s="8" t="n">
-        <v>45874</v>
-      </c>
+      <c r="A179" s="8"/>
+      <c r="B179" s="8"/>
       <c r="C179" s="8"/>
     </row>
     <row r="180" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A180" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B180" s="8" t="n">
-        <v>45874</v>
-      </c>
+      <c r="A180" s="8"/>
+      <c r="B180" s="8"/>
       <c r="C180" s="8"/>
     </row>
     <row r="181" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A181" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B181" s="8" t="n">
-        <v>45873</v>
-      </c>
+      <c r="A181" s="8"/>
+      <c r="B181" s="8"/>
       <c r="C181" s="8"/>
     </row>
     <row r="182" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A182" s="8" t="n">
-        <v>45878</v>
-      </c>
-      <c r="B182" s="8" t="n">
-        <v>45879</v>
-      </c>
+      <c r="A182" s="8"/>
+      <c r="B182" s="8"/>
       <c r="C182" s="8"/>
     </row>
     <row r="183" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A183" s="8" t="n">
-        <v>45875</v>
-      </c>
-      <c r="B183" s="8" t="n">
-        <v>45876</v>
-      </c>
+      <c r="A183" s="8"/>
+      <c r="B183" s="8"/>
       <c r="C183" s="8"/>
     </row>
     <row r="184" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A184" s="8" t="n">
-        <v>45878</v>
-      </c>
-      <c r="B184" s="8" t="n">
-        <v>45879</v>
-      </c>
+      <c r="A184" s="8"/>
+      <c r="B184" s="8"/>
       <c r="C184" s="8"/>
     </row>
     <row r="185" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A185" s="8" t="n">
-        <v>45877</v>
-      </c>
-      <c r="B185" s="8" t="n">
-        <v>45878</v>
-      </c>
+      <c r="A185" s="8"/>
+      <c r="B185" s="8"/>
       <c r="C185" s="8"/>
     </row>
     <row r="186" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A186" s="8" t="n">
-        <v>45877</v>
-      </c>
-      <c r="B186" s="8" t="n">
-        <v>45878</v>
-      </c>
+      <c r="A186" s="8"/>
+      <c r="B186" s="8"/>
       <c r="C186" s="8"/>
     </row>
     <row r="187" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A187" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B187" s="8" t="n">
-        <v>45873</v>
-      </c>
+      <c r="A187" s="8"/>
+      <c r="B187" s="8"/>
       <c r="C187" s="8"/>
     </row>
     <row r="188" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A188" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B188" s="8" t="n">
-        <v>45875</v>
-      </c>
+      <c r="A188" s="8"/>
+      <c r="B188" s="8"/>
       <c r="C188" s="8"/>
     </row>
     <row r="189" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A189" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B189" s="8" t="n">
-        <v>45874</v>
-      </c>
+      <c r="A189" s="8"/>
+      <c r="B189" s="8"/>
       <c r="C189" s="8"/>
     </row>
     <row r="190" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A190" s="8" t="n">
-        <v>45870</v>
-      </c>
-      <c r="B190" s="8" t="n">
-        <v>45871</v>
-      </c>
+      <c r="A190" s="8"/>
+      <c r="B190" s="8"/>
       <c r="C190" s="8"/>
     </row>
     <row r="191" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A191" s="8" t="n">
-        <v>45870</v>
-      </c>
-      <c r="B191" s="8" t="n">
-        <v>45870</v>
-      </c>
+      <c r="A191" s="8"/>
+      <c r="B191" s="8"/>
       <c r="C191" s="8"/>
     </row>
     <row r="192" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A192" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B192" s="8" t="n">
-        <v>45875</v>
-      </c>
+      <c r="A192" s="8"/>
+      <c r="B192" s="8"/>
       <c r="C192" s="8"/>
     </row>
     <row r="193" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A193" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B193" s="8" t="n">
-        <v>45875</v>
-      </c>
+      <c r="A193" s="8"/>
+      <c r="B193" s="8"/>
       <c r="C193" s="8"/>
     </row>
     <row r="194" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A194" s="8" t="n">
-        <v>45871</v>
-      </c>
-      <c r="B194" s="8" t="n">
-        <v>45872</v>
-      </c>
+      <c r="A194" s="8"/>
+      <c r="B194" s="8"/>
       <c r="C194" s="8"/>
     </row>
     <row r="195" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A195" s="4" t="n">
-        <v>45880</v>
-      </c>
-      <c r="B195" s="4" t="n">
-        <v>45881</v>
-      </c>
+      <c r="A195" s="4"/>
+      <c r="B195" s="4"/>
       <c r="C195" s="4"/>
     </row>
     <row r="196" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A196" s="8" t="n">
-        <v>45878</v>
-      </c>
-      <c r="B196" s="8" t="n">
-        <v>45879</v>
-      </c>
+      <c r="A196" s="8"/>
+      <c r="B196" s="8"/>
       <c r="C196" s="8"/>
     </row>
     <row r="197" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A197" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B197" s="8" t="n">
-        <v>45875</v>
-      </c>
+      <c r="A197" s="8"/>
+      <c r="B197" s="8"/>
       <c r="C197" s="8"/>
     </row>
     <row r="198" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A198" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B198" s="8" t="n">
-        <v>45873</v>
-      </c>
+      <c r="A198" s="8"/>
+      <c r="B198" s="8"/>
       <c r="C198" s="8"/>
     </row>
     <row r="199" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A199" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B199" s="8" t="n">
-        <v>45875</v>
-      </c>
+      <c r="A199" s="8"/>
+      <c r="B199" s="8"/>
       <c r="C199" s="8"/>
     </row>
     <row r="200" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A200" s="8" t="n">
-        <v>45870</v>
-      </c>
-      <c r="B200" s="8" t="n">
-        <v>45873</v>
-      </c>
+      <c r="A200" s="8"/>
+      <c r="B200" s="8"/>
       <c r="C200" s="8"/>
     </row>
     <row r="201" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A201" s="4" t="n">
-        <v>45879</v>
-      </c>
-      <c r="B201" s="4" t="n">
-        <v>45880</v>
-      </c>
+      <c r="A201" s="4"/>
+      <c r="B201" s="4"/>
       <c r="C201" s="4"/>
     </row>
     <row r="202" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A202" s="8" t="n">
-        <v>45876</v>
-      </c>
-      <c r="B202" s="8" t="n">
-        <v>45877</v>
-      </c>
+      <c r="A202" s="8"/>
+      <c r="B202" s="8"/>
       <c r="C202" s="8"/>
     </row>
     <row r="203" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A203" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B203" s="8" t="n">
-        <v>45875</v>
-      </c>
+      <c r="A203" s="8"/>
+      <c r="B203" s="8"/>
       <c r="C203" s="8"/>
     </row>
     <row r="204" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A204" s="8" t="n">
-        <v>45876</v>
-      </c>
-      <c r="B204" s="8" t="n">
-        <v>45877</v>
-      </c>
+      <c r="A204" s="8"/>
+      <c r="B204" s="8"/>
       <c r="C204" s="8"/>
     </row>
     <row r="205" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A205" s="13" t="n">
-        <v>45869</v>
-      </c>
-      <c r="B205" s="13" t="n">
-        <v>45870</v>
-      </c>
-      <c r="C205" s="13"/>
+      <c r="A205" s="17"/>
+      <c r="B205" s="17"/>
+      <c r="C205" s="17"/>
     </row>
     <row r="206" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A206" s="13" t="n">
-        <v>45869</v>
-      </c>
-      <c r="B206" s="13" t="n">
-        <v>45870</v>
-      </c>
-      <c r="C206" s="13"/>
+      <c r="A206" s="17"/>
+      <c r="B206" s="17"/>
+      <c r="C206" s="17"/>
     </row>
     <row r="207" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A207" s="8" t="n">
-        <v>45876</v>
-      </c>
-      <c r="B207" s="8" t="n">
-        <v>45876</v>
-      </c>
+      <c r="A207" s="8"/>
+      <c r="B207" s="8"/>
       <c r="C207" s="8"/>
     </row>
     <row r="208" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A208" s="8" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B208" s="8" t="n">
-        <v>45874</v>
-      </c>
+      <c r="A208" s="8"/>
+      <c r="B208" s="8"/>
       <c r="C208" s="8"/>
     </row>
     <row r="209" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A209" s="4" t="n">
-        <v>45879</v>
-      </c>
-      <c r="B209" s="4" t="n">
-        <v>45880</v>
-      </c>
+      <c r="A209" s="4"/>
+      <c r="B209" s="4"/>
       <c r="C209" s="4"/>
     </row>
     <row r="210" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A210" s="8" t="n">
-        <v>45878</v>
-      </c>
-      <c r="B210" s="8" t="n">
-        <v>45879</v>
-      </c>
+      <c r="A210" s="8"/>
+      <c r="B210" s="8"/>
       <c r="C210" s="8"/>
     </row>
     <row r="211" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A211" s="8" t="n">
-        <v>45877</v>
-      </c>
-      <c r="B211" s="8" t="n">
-        <v>45878</v>
-      </c>
+      <c r="A211" s="8"/>
+      <c r="B211" s="8"/>
       <c r="C211" s="8"/>
     </row>
     <row r="212" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A212" s="8" t="n">
-        <v>45872</v>
-      </c>
-      <c r="B212" s="8" t="n">
-        <v>45873</v>
-      </c>
+      <c r="A212" s="8"/>
+      <c r="B212" s="8"/>
       <c r="C212" s="8"/>
     </row>
     <row r="213" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A213" s="8" t="n">
-        <v>45870</v>
-      </c>
-      <c r="B213" s="8" t="n">
-        <v>45871</v>
-      </c>
+      <c r="A213" s="8"/>
+      <c r="B213" s="8"/>
       <c r="C213" s="8"/>
     </row>
     <row r="214" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A214" s="8" t="n">
-        <v>45870</v>
-      </c>
-      <c r="B214" s="8" t="n">
-        <v>45871</v>
-      </c>
+      <c r="A214" s="8"/>
+      <c r="B214" s="8"/>
       <c r="C214" s="8"/>
     </row>
     <row r="215" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A215" s="8" t="n">
-        <v>45871</v>
-      </c>
-      <c r="B215" s="8" t="n">
-        <v>45872</v>
-      </c>
+      <c r="A215" s="8"/>
+      <c r="B215" s="8"/>
       <c r="C215" s="8"/>
     </row>
     <row r="216" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A216" s="8" t="n">
-        <v>45875</v>
-      </c>
-      <c r="B216" s="8" t="n">
-        <v>45877</v>
-      </c>
+      <c r="A216" s="8"/>
+      <c r="B216" s="8"/>
       <c r="C216" s="8"/>
     </row>
     <row r="217" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A217" s="4" t="n">
-        <v>45880</v>
-      </c>
-      <c r="B217" s="4" t="n">
-        <v>45881</v>
-      </c>
+      <c r="A217" s="4"/>
+      <c r="B217" s="4"/>
       <c r="C217" s="4"/>
     </row>
     <row r="218" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A218" s="4" t="n">
-        <v>45880</v>
-      </c>
-      <c r="B218" s="4" t="n">
-        <v>45881</v>
-      </c>
+      <c r="A218" s="4"/>
+      <c r="B218" s="4"/>
       <c r="C218" s="4"/>
     </row>
     <row r="219" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A219" s="8" t="n">
-        <v>45876</v>
-      </c>
-      <c r="B219" s="8" t="n">
-        <v>45877</v>
-      </c>
+      <c r="A219" s="8"/>
+      <c r="B219" s="8"/>
       <c r="C219" s="8"/>
     </row>
     <row r="220" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A220" s="8" t="n">
-        <v>45875</v>
-      </c>
-      <c r="B220" s="8" t="n">
-        <v>45876</v>
-      </c>
+      <c r="A220" s="8"/>
+      <c r="B220" s="8"/>
       <c r="C220" s="8"/>
     </row>
     <row r="221" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A221" s="8" t="n">
-        <v>45871</v>
-      </c>
-      <c r="B221" s="8" t="n">
-        <v>45872</v>
-      </c>
+      <c r="A221" s="8"/>
+      <c r="B221" s="8"/>
       <c r="C221" s="8"/>
     </row>
     <row r="222" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A222" s="8" t="n">
-        <v>45877</v>
-      </c>
-      <c r="B222" s="8" t="n">
-        <v>45878</v>
-      </c>
+      <c r="A222" s="8"/>
+      <c r="B222" s="8"/>
       <c r="C222" s="8"/>
     </row>
     <row r="223" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A223" s="8" t="n">
-        <v>45870</v>
-      </c>
-      <c r="B223" s="8" t="n">
-        <v>45871</v>
-      </c>
+      <c r="A223" s="8"/>
+      <c r="B223" s="8"/>
       <c r="C223" s="8"/>
     </row>
     <row r="224" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A224" s="8" t="n">
-        <v>45879</v>
-      </c>
-      <c r="B224" s="8" t="n">
-        <v>45879</v>
-      </c>
+      <c r="A224" s="8"/>
+      <c r="B224" s="8"/>
       <c r="C224" s="8"/>
     </row>
     <row r="225" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A225" s="8" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B225" s="8" t="n">
-        <v>45874</v>
-      </c>
+      <c r="A225" s="8"/>
+      <c r="B225" s="8"/>
       <c r="C225" s="8"/>
     </row>
     <row r="226" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A226" s="4" t="n">
-        <v>45879</v>
-      </c>
-      <c r="B226" s="4" t="n">
-        <v>45880</v>
-      </c>
+      <c r="A226" s="4"/>
+      <c r="B226" s="4"/>
       <c r="C226" s="4"/>
     </row>
     <row r="227" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A227" s="8" t="n">
-        <v>45871</v>
-      </c>
-      <c r="B227" s="8" t="n">
-        <v>45872</v>
-      </c>
+      <c r="A227" s="8"/>
+      <c r="B227" s="8"/>
       <c r="C227" s="8"/>
     </row>
+    <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <autoFilter ref="A1:P2"/>
   <mergeCells count="4">

</xml_diff>